<commit_message>
Refactor to combine genotype and treatment comparisons into single compare_groups functions
</commit_message>
<xml_diff>
--- a/inst/extdata/example-genotype.xlsx
+++ b/inst/extdata/example-genotype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mctools-my.sharepoint.com/personal/lindsey_richard_mayo_edu/Documents/Lab/microCTr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{7A772ADF-69BF-4A71-99C1-38E30A0CE021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42235D44-0AF1-4624-94DD-419B9B670D34}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{7A772ADF-69BF-4A71-99C1-38E30A0CE021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78F3A6DF-2FCC-4788-B692-2EB2E4E5E0EA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6894D22F-2E2C-44C1-B8A7-16983EAC7257}"/>
   </bookViews>
@@ -4380,12 +4380,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5088,7 +5090,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
+    <col min="21" max="21" width="9.140625" style="6"/>
+    <col min="22" max="22" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="24" max="27" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -5153,10 +5156,10 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -5371,10 +5374,10 @@
       <c r="T2">
         <v>2.5285000000000002</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="6">
         <v>0.13719999999999999</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="W2">
@@ -5583,10 +5586,10 @@
       <c r="T3">
         <v>2.5293000000000001</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="6">
         <v>0.3301</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="4">
         <v>0.1305</v>
       </c>
       <c r="W3">
@@ -5795,10 +5798,10 @@
       <c r="T4">
         <v>0.2203</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="6">
         <v>4.82E-2</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>0.21879999999999999</v>
       </c>
       <c r="W4">
@@ -6007,10 +6010,10 @@
       <c r="T5">
         <v>2.1027</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="6">
         <v>0.30420000000000003</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="4">
         <v>0.1447</v>
       </c>
       <c r="W5">
@@ -6219,10 +6222,10 @@
       <c r="T6">
         <v>2.4906999999999999</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="6">
         <v>0.4995</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="4">
         <v>0.2006</v>
       </c>
       <c r="W6">
@@ -6431,10 +6434,10 @@
       <c r="T7">
         <v>2.7296999999999998</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="6">
         <v>0.62490000000000001</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="4">
         <v>0.22889999999999999</v>
       </c>
       <c r="W7">
@@ -6643,10 +6646,10 @@
       <c r="T8">
         <v>1.5992</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="6">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="4">
         <v>4.4699999999999997E-2</v>
       </c>
       <c r="W8">
@@ -6855,10 +6858,10 @@
       <c r="T9">
         <v>2.4661</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="6">
         <v>0.5262</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="4">
         <v>0.21340000000000001</v>
       </c>
       <c r="W9">
@@ -7067,10 +7070,10 @@
       <c r="T10">
         <v>2.4327000000000001</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="6">
         <v>0.4088</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="4">
         <v>0.16800000000000001</v>
       </c>
       <c r="W10">
@@ -7279,10 +7282,10 @@
       <c r="T11">
         <v>2.4535</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="6">
         <v>0.40329999999999999</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="4">
         <v>0.16439999999999999</v>
       </c>
       <c r="W11">
@@ -7491,10 +7494,10 @@
       <c r="T12">
         <v>2.3399000000000001</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12" s="6">
         <v>0.38600000000000001</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="4">
         <v>0.16500000000000001</v>
       </c>
       <c r="W12">
@@ -7703,10 +7706,10 @@
       <c r="T13">
         <v>1.8832</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="6">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="4">
         <v>2.3E-3</v>
       </c>
       <c r="W13">
@@ -7915,10 +7918,10 @@
       <c r="T14">
         <v>1.6694</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="6">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="4">
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="W14">
@@ -8127,10 +8130,10 @@
       <c r="T15">
         <v>2.1495000000000002</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="6">
         <v>0.26929999999999998</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="4">
         <v>0.12529999999999999</v>
       </c>
       <c r="W15">
@@ -8339,10 +8342,10 @@
       <c r="T16">
         <v>2.0682</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16" s="6">
         <v>0.13220000000000001</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="4">
         <v>6.3899999999999998E-2</v>
       </c>
       <c r="W16">
@@ -8551,10 +8554,10 @@
       <c r="T17">
         <v>1.3996</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U17" s="6">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="4">
         <v>1.6199999999999999E-2</v>
       </c>
       <c r="W17">
@@ -8763,10 +8766,10 @@
       <c r="T18">
         <v>1.5076000000000001</v>
       </c>
-      <c r="U18" s="4">
+      <c r="U18" s="6">
         <v>2.01E-2</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="4">
         <v>1.3299999999999999E-2</v>
       </c>
       <c r="W18">
@@ -8975,10 +8978,10 @@
       <c r="T19">
         <v>1.2110000000000001</v>
       </c>
-      <c r="U19" s="4">
+      <c r="U19" s="6">
         <v>2.75E-2</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="4">
         <v>2.2700000000000001E-2</v>
       </c>
       <c r="W19">
@@ -9187,10 +9190,10 @@
       <c r="T20">
         <v>2.6455000000000002</v>
       </c>
-      <c r="U20" s="4">
+      <c r="U20" s="6">
         <v>0.43149999999999999</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="4">
         <v>0.16309999999999999</v>
       </c>
       <c r="W20">
@@ -9399,10 +9402,10 @@
       <c r="T21">
         <v>2.2869000000000002</v>
       </c>
-      <c r="U21" s="4">
+      <c r="U21" s="6">
         <v>0.4677</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="4">
         <v>0.20449999999999999</v>
       </c>
       <c r="W21">
@@ -9611,10 +9614,10 @@
       <c r="T22">
         <v>2.5779999999999998</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U22" s="6">
         <v>0.54479999999999995</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="4">
         <v>0.21129999999999999</v>
       </c>
       <c r="W22">
@@ -9823,10 +9826,10 @@
       <c r="T23">
         <v>2.0771000000000002</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U23" s="6">
         <v>0.13669999999999999</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="4">
         <v>6.5799999999999997E-2</v>
       </c>
       <c r="W23">
@@ -10035,10 +10038,10 @@
       <c r="T24">
         <v>1.9416</v>
       </c>
-      <c r="U24" s="4">
+      <c r="U24" s="6">
         <v>0.28549999999999998</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="4">
         <v>0.14699999999999999</v>
       </c>
       <c r="W24">
@@ -10247,10 +10250,10 @@
       <c r="T25">
         <v>1.9458</v>
       </c>
-      <c r="U25" s="4">
+      <c r="U25" s="6">
         <v>0.16839999999999999</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="4">
         <v>8.6499999999999994E-2</v>
       </c>
       <c r="W25">

</xml_diff>